<commit_message>
Graph wasn't bidirectional, was causing issues
</commit_message>
<xml_diff>
--- a/bipartite_matching/bmGraph.xlsx
+++ b/bipartite_matching/bmGraph.xlsx
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,17 +455,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -542,6 +538,78 @@
       </c>
       <c r="B10">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>